<commit_message>
upload: added data files
</commit_message>
<xml_diff>
--- a/data/2024년 1학기 정규 시간표.xlsx
+++ b/data/2024년 1학기 정규 시간표.xlsx
@@ -5669,7 +5669,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>임선영</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
@@ -5865,7 +5865,7 @@
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>미지정</t>
+          <t>박정화</t>
         </is>
       </c>
       <c r="J89" t="inlineStr"/>
@@ -8655,7 +8655,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I136" t="inlineStr"/>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>정인</t>
+        </is>
+      </c>
       <c r="J136" t="inlineStr">
         <is>
           <t>금2~4</t>
@@ -8827,7 +8831,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I139" t="inlineStr"/>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>최담선</t>
+        </is>
+      </c>
       <c r="J139" t="inlineStr">
         <is>
           <t>금6~8</t>
@@ -13642,7 +13650,7 @@
       <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr">
         <is>
-          <t>월1~2</t>
+          <t>월2~3</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
@@ -13696,8 +13704,16 @@
         </is>
       </c>
       <c r="I221" t="inlineStr"/>
-      <c r="J221" t="inlineStr"/>
-      <c r="K221" t="inlineStr"/>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>월4~5</t>
+        </is>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L221" t="inlineStr">
         <is>
           <t>과학기술대학</t>
@@ -13859,7 +13875,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I224" t="inlineStr"/>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>이재환</t>
+        </is>
+      </c>
       <c r="J224" t="inlineStr">
         <is>
           <t>목1~3</t>
@@ -14098,7 +14118,7 @@
       <c r="I228" t="inlineStr"/>
       <c r="J228" t="inlineStr">
         <is>
-          <t>월4~5</t>
+          <t>수2~3</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
@@ -14154,7 +14174,7 @@
       <c r="I229" t="inlineStr"/>
       <c r="J229" t="inlineStr">
         <is>
-          <t>월1~2</t>
+          <t>화1~2</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
@@ -15475,7 +15495,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I251" t="inlineStr"/>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>김영준</t>
+        </is>
+      </c>
       <c r="J251" t="inlineStr">
         <is>
           <t>목1~3</t>
@@ -15591,7 +15615,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I253" t="inlineStr"/>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>태종욱</t>
+        </is>
+      </c>
       <c r="J253" t="inlineStr">
         <is>
           <t>수5~7</t>
@@ -15887,7 +15915,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I258" t="inlineStr"/>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>양형모</t>
+        </is>
+      </c>
       <c r="J258" t="inlineStr">
         <is>
           <t>목5~7</t>
@@ -16363,7 +16395,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I266" t="inlineStr"/>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>김영준</t>
+        </is>
+      </c>
       <c r="J266" t="inlineStr">
         <is>
           <t>목5~7</t>
@@ -16419,7 +16455,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I267" t="inlineStr"/>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>양형모</t>
+        </is>
+      </c>
       <c r="J267" t="inlineStr">
         <is>
           <t>목1~3</t>
@@ -36795,7 +36835,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="I604" t="inlineStr"/>
+      <c r="I604" t="inlineStr">
+        <is>
+          <t>김주연</t>
+        </is>
+      </c>
       <c r="J604" t="inlineStr">
         <is>
           <t>수6~8</t>
@@ -52737,11 +52781,19 @@
       </c>
       <c r="I870" t="inlineStr">
         <is>
-          <t>이재구</t>
-        </is>
-      </c>
-      <c r="J870" t="inlineStr"/>
-      <c r="K870" t="inlineStr"/>
+          <t>유재현</t>
+        </is>
+      </c>
+      <c r="J870" t="inlineStr">
+        <is>
+          <t>목1~3</t>
+        </is>
+      </c>
+      <c r="K870" t="inlineStr">
+        <is>
+          <t>체육관309호(中)강의실</t>
+        </is>
+      </c>
       <c r="L870" t="inlineStr">
         <is>
           <t>보건복지대학</t>
@@ -52789,11 +52841,19 @@
       </c>
       <c r="I871" t="inlineStr">
         <is>
-          <t>김우겸</t>
-        </is>
-      </c>
-      <c r="J871" t="inlineStr"/>
-      <c r="K871" t="inlineStr"/>
+          <t>미지정</t>
+        </is>
+      </c>
+      <c r="J871" t="inlineStr">
+        <is>
+          <t>금3~4</t>
+        </is>
+      </c>
+      <c r="K871" t="inlineStr">
+        <is>
+          <t>체육관203호(주경기장)</t>
+        </is>
+      </c>
       <c r="L871" t="inlineStr">
         <is>
           <t>보건복지대학</t>
@@ -88800,8 +88860,16 @@
           <t>김영수</t>
         </is>
       </c>
-      <c r="J1443" t="inlineStr"/>
-      <c r="K1443" t="inlineStr"/>
+      <c r="J1443" t="inlineStr">
+        <is>
+          <t>화8</t>
+        </is>
+      </c>
+      <c r="K1443" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1443" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -88852,8 +88920,16 @@
           <t>김영수</t>
         </is>
       </c>
-      <c r="J1444" t="inlineStr"/>
-      <c r="K1444" t="inlineStr"/>
+      <c r="J1444" t="inlineStr">
+        <is>
+          <t>월3</t>
+        </is>
+      </c>
+      <c r="K1444" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1444" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -88904,8 +88980,16 @@
           <t>김영수</t>
         </is>
       </c>
-      <c r="J1445" t="inlineStr"/>
-      <c r="K1445" t="inlineStr"/>
+      <c r="J1445" t="inlineStr">
+        <is>
+          <t>수2</t>
+        </is>
+      </c>
+      <c r="K1445" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1445" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -88956,8 +89040,16 @@
           <t>이효성</t>
         </is>
       </c>
-      <c r="J1446" t="inlineStr"/>
-      <c r="K1446" t="inlineStr"/>
+      <c r="J1446" t="inlineStr">
+        <is>
+          <t>화9</t>
+        </is>
+      </c>
+      <c r="K1446" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1446" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89008,8 +89100,16 @@
           <t>김민주</t>
         </is>
       </c>
-      <c r="J1447" t="inlineStr"/>
-      <c r="K1447" t="inlineStr"/>
+      <c r="J1447" t="inlineStr">
+        <is>
+          <t>화9</t>
+        </is>
+      </c>
+      <c r="K1447" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1447" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89060,8 +89160,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J1448" t="inlineStr"/>
-      <c r="K1448" t="inlineStr"/>
+      <c r="J1448" t="inlineStr">
+        <is>
+          <t>화9</t>
+        </is>
+      </c>
+      <c r="K1448" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1448" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89112,8 +89220,16 @@
           <t>유예진</t>
         </is>
       </c>
-      <c r="J1449" t="inlineStr"/>
-      <c r="K1449" t="inlineStr"/>
+      <c r="J1449" t="inlineStr">
+        <is>
+          <t>화9</t>
+        </is>
+      </c>
+      <c r="K1449" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1449" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89160,8 +89276,16 @@
         </is>
       </c>
       <c r="I1450" t="inlineStr"/>
-      <c r="J1450" t="inlineStr"/>
-      <c r="K1450" t="inlineStr"/>
+      <c r="J1450" t="inlineStr">
+        <is>
+          <t>화9</t>
+        </is>
+      </c>
+      <c r="K1450" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1450" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89216,8 +89340,16 @@
           <t>김영수</t>
         </is>
       </c>
-      <c r="J1451" t="inlineStr"/>
-      <c r="K1451" t="inlineStr"/>
+      <c r="J1451" t="inlineStr">
+        <is>
+          <t>월6~7</t>
+        </is>
+      </c>
+      <c r="K1451" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1451" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89328,8 +89460,16 @@
           <t>유예진</t>
         </is>
       </c>
-      <c r="J1453" t="inlineStr"/>
-      <c r="K1453" t="inlineStr"/>
+      <c r="J1453" t="inlineStr">
+        <is>
+          <t>목6~8</t>
+        </is>
+      </c>
+      <c r="K1453" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1453" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89380,8 +89520,16 @@
           <t>신용재</t>
         </is>
       </c>
-      <c r="J1454" t="inlineStr"/>
-      <c r="K1454" t="inlineStr"/>
+      <c r="J1454" t="inlineStr">
+        <is>
+          <t>목2~4</t>
+        </is>
+      </c>
+      <c r="K1454" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1454" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89428,8 +89576,16 @@
         </is>
       </c>
       <c r="I1455" t="inlineStr"/>
-      <c r="J1455" t="inlineStr"/>
-      <c r="K1455" t="inlineStr"/>
+      <c r="J1455" t="inlineStr">
+        <is>
+          <t>화2~4</t>
+        </is>
+      </c>
+      <c r="K1455" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1455" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89480,8 +89636,16 @@
           <t>민세원</t>
         </is>
       </c>
-      <c r="J1456" t="inlineStr"/>
-      <c r="K1456" t="inlineStr"/>
+      <c r="J1456" t="inlineStr">
+        <is>
+          <t>수6~8</t>
+        </is>
+      </c>
+      <c r="K1456" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1456" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89536,8 +89700,16 @@
           <t>김영수</t>
         </is>
       </c>
-      <c r="J1457" t="inlineStr"/>
-      <c r="K1457" t="inlineStr"/>
+      <c r="J1457" t="inlineStr">
+        <is>
+          <t>월6~7</t>
+        </is>
+      </c>
+      <c r="K1457" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1457" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89592,8 +89764,16 @@
           <t>이효성</t>
         </is>
       </c>
-      <c r="J1458" t="inlineStr"/>
-      <c r="K1458" t="inlineStr"/>
+      <c r="J1458" t="inlineStr">
+        <is>
+          <t>화2~4</t>
+        </is>
+      </c>
+      <c r="K1458" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1458" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89644,8 +89824,16 @@
           <t>KITAUCHI DAITO</t>
         </is>
       </c>
-      <c r="J1459" t="inlineStr"/>
-      <c r="K1459" t="inlineStr"/>
+      <c r="J1459" t="inlineStr">
+        <is>
+          <t>수1~3</t>
+        </is>
+      </c>
+      <c r="K1459" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1459" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89696,8 +89884,16 @@
           <t>유예진</t>
         </is>
       </c>
-      <c r="J1460" t="inlineStr"/>
-      <c r="K1460" t="inlineStr"/>
+      <c r="J1460" t="inlineStr">
+        <is>
+          <t>화6~8</t>
+        </is>
+      </c>
+      <c r="K1460" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1460" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89744,8 +89940,16 @@
         </is>
       </c>
       <c r="I1461" t="inlineStr"/>
-      <c r="J1461" t="inlineStr"/>
-      <c r="K1461" t="inlineStr"/>
+      <c r="J1461" t="inlineStr">
+        <is>
+          <t>금2~4</t>
+        </is>
+      </c>
+      <c r="K1461" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1461" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89796,8 +90000,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J1462" t="inlineStr"/>
-      <c r="K1462" t="inlineStr"/>
+      <c r="J1462" t="inlineStr">
+        <is>
+          <t>목2~4</t>
+        </is>
+      </c>
+      <c r="K1462" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1462" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89844,8 +90056,16 @@
         </is>
       </c>
       <c r="I1463" t="inlineStr"/>
-      <c r="J1463" t="inlineStr"/>
-      <c r="K1463" t="inlineStr"/>
+      <c r="J1463" t="inlineStr">
+        <is>
+          <t>수2~4</t>
+        </is>
+      </c>
+      <c r="K1463" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1463" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89896,8 +90116,16 @@
           <t>김민주</t>
         </is>
       </c>
-      <c r="J1464" t="inlineStr"/>
-      <c r="K1464" t="inlineStr"/>
+      <c r="J1464" t="inlineStr">
+        <is>
+          <t>목6~8</t>
+        </is>
+      </c>
+      <c r="K1464" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1464" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -89948,8 +90176,16 @@
           <t>민세원</t>
         </is>
       </c>
-      <c r="J1465" t="inlineStr"/>
-      <c r="K1465" t="inlineStr"/>
+      <c r="J1465" t="inlineStr">
+        <is>
+          <t>금2~4</t>
+        </is>
+      </c>
+      <c r="K1465" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1465" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90000,8 +90236,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J1466" t="inlineStr"/>
-      <c r="K1466" t="inlineStr"/>
+      <c r="J1466" t="inlineStr">
+        <is>
+          <t>월6~8</t>
+        </is>
+      </c>
+      <c r="K1466" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1466" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90052,8 +90296,16 @@
           <t>장성숙</t>
         </is>
       </c>
-      <c r="J1467" t="inlineStr"/>
-      <c r="K1467" t="inlineStr"/>
+      <c r="J1467" t="inlineStr">
+        <is>
+          <t>화8~10</t>
+        </is>
+      </c>
+      <c r="K1467" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1467" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90104,8 +90356,16 @@
           <t>김민주</t>
         </is>
       </c>
-      <c r="J1468" t="inlineStr"/>
-      <c r="K1468" t="inlineStr"/>
+      <c r="J1468" t="inlineStr">
+        <is>
+          <t>수3~5</t>
+        </is>
+      </c>
+      <c r="K1468" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1468" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90156,8 +90416,16 @@
           <t>유예진</t>
         </is>
       </c>
-      <c r="J1469" t="inlineStr"/>
-      <c r="K1469" t="inlineStr"/>
+      <c r="J1469" t="inlineStr">
+        <is>
+          <t>화2~4</t>
+        </is>
+      </c>
+      <c r="K1469" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1469" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90208,8 +90476,16 @@
           <t>KITAUCHI DAITO</t>
         </is>
       </c>
-      <c r="J1470" t="inlineStr"/>
-      <c r="K1470" t="inlineStr"/>
+      <c r="J1470" t="inlineStr">
+        <is>
+          <t>월1~3</t>
+        </is>
+      </c>
+      <c r="K1470" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1470" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90256,8 +90532,16 @@
         </is>
       </c>
       <c r="I1471" t="inlineStr"/>
-      <c r="J1471" t="inlineStr"/>
-      <c r="K1471" t="inlineStr"/>
+      <c r="J1471" t="inlineStr">
+        <is>
+          <t>수6~8</t>
+        </is>
+      </c>
+      <c r="K1471" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1471" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90308,8 +90592,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J1472" t="inlineStr"/>
-      <c r="K1472" t="inlineStr"/>
+      <c r="J1472" t="inlineStr">
+        <is>
+          <t>목6~8</t>
+        </is>
+      </c>
+      <c r="K1472" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1472" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90360,8 +90652,16 @@
           <t>김민주</t>
         </is>
       </c>
-      <c r="J1473" t="inlineStr"/>
-      <c r="K1473" t="inlineStr"/>
+      <c r="J1473" t="inlineStr">
+        <is>
+          <t>목2~4</t>
+        </is>
+      </c>
+      <c r="K1473" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1473" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90412,8 +90712,16 @@
           <t>이효성</t>
         </is>
       </c>
-      <c r="J1474" t="inlineStr"/>
-      <c r="K1474" t="inlineStr"/>
+      <c r="J1474" t="inlineStr">
+        <is>
+          <t>금6~8</t>
+        </is>
+      </c>
+      <c r="K1474" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1474" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90464,8 +90772,16 @@
           <t>김영수</t>
         </is>
       </c>
-      <c r="J1475" t="inlineStr"/>
-      <c r="K1475" t="inlineStr"/>
+      <c r="J1475" t="inlineStr">
+        <is>
+          <t>월9</t>
+        </is>
+      </c>
+      <c r="K1475" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1475" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90516,8 +90832,16 @@
           <t>민세원</t>
         </is>
       </c>
-      <c r="J1476" t="inlineStr"/>
-      <c r="K1476" t="inlineStr"/>
+      <c r="J1476" t="inlineStr">
+        <is>
+          <t>월2~4</t>
+        </is>
+      </c>
+      <c r="K1476" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1476" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90568,8 +90892,16 @@
           <t>민세원</t>
         </is>
       </c>
-      <c r="J1477" t="inlineStr"/>
-      <c r="K1477" t="inlineStr"/>
+      <c r="J1477" t="inlineStr">
+        <is>
+          <t>월6~8</t>
+        </is>
+      </c>
+      <c r="K1477" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1477" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90620,8 +90952,16 @@
           <t>이효성</t>
         </is>
       </c>
-      <c r="J1478" t="inlineStr"/>
-      <c r="K1478" t="inlineStr"/>
+      <c r="J1478" t="inlineStr">
+        <is>
+          <t>금2~4</t>
+        </is>
+      </c>
+      <c r="K1478" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1478" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90672,8 +91012,16 @@
           <t>김남경</t>
         </is>
       </c>
-      <c r="J1479" t="inlineStr"/>
-      <c r="K1479" t="inlineStr"/>
+      <c r="J1479" t="inlineStr">
+        <is>
+          <t>수2~4</t>
+        </is>
+      </c>
+      <c r="K1479" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1479" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90724,8 +91072,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J1480" t="inlineStr"/>
-      <c r="K1480" t="inlineStr"/>
+      <c r="J1480" t="inlineStr">
+        <is>
+          <t>화2~4</t>
+        </is>
+      </c>
+      <c r="K1480" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1480" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90776,8 +91132,16 @@
           <t>유예진</t>
         </is>
       </c>
-      <c r="J1481" t="inlineStr"/>
-      <c r="K1481" t="inlineStr"/>
+      <c r="J1481" t="inlineStr">
+        <is>
+          <t>목2~4</t>
+        </is>
+      </c>
+      <c r="K1481" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1481" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90828,8 +91192,16 @@
           <t>안병삼</t>
         </is>
       </c>
-      <c r="J1482" t="inlineStr"/>
-      <c r="K1482" t="inlineStr"/>
+      <c r="J1482" t="inlineStr">
+        <is>
+          <t>화6~8</t>
+        </is>
+      </c>
+      <c r="K1482" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1482" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90880,8 +91252,16 @@
           <t>장성숙</t>
         </is>
       </c>
-      <c r="J1483" t="inlineStr"/>
-      <c r="K1483" t="inlineStr"/>
+      <c r="J1483" t="inlineStr">
+        <is>
+          <t>화11~13</t>
+        </is>
+      </c>
+      <c r="K1483" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1483" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90928,8 +91308,16 @@
         </is>
       </c>
       <c r="I1484" t="inlineStr"/>
-      <c r="J1484" t="inlineStr"/>
-      <c r="K1484" t="inlineStr"/>
+      <c r="J1484" t="inlineStr">
+        <is>
+          <t>금8~10</t>
+        </is>
+      </c>
+      <c r="K1484" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1484" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -90976,8 +91364,16 @@
         </is>
       </c>
       <c r="I1485" t="inlineStr"/>
-      <c r="J1485" t="inlineStr"/>
-      <c r="K1485" t="inlineStr"/>
+      <c r="J1485" t="inlineStr">
+        <is>
+          <t>목6~8</t>
+        </is>
+      </c>
+      <c r="K1485" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1485" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -91028,8 +91424,16 @@
           <t>김민주</t>
         </is>
       </c>
-      <c r="J1486" t="inlineStr"/>
-      <c r="K1486" t="inlineStr"/>
+      <c r="J1486" t="inlineStr">
+        <is>
+          <t>화6~8</t>
+        </is>
+      </c>
+      <c r="K1486" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1486" t="inlineStr">
         <is>
           <t>인문사회대학</t>
@@ -91080,8 +91484,16 @@
           <t>김민주</t>
         </is>
       </c>
-      <c r="J1487" t="inlineStr"/>
-      <c r="K1487" t="inlineStr"/>
+      <c r="J1487" t="inlineStr">
+        <is>
+          <t>화6~8</t>
+        </is>
+      </c>
+      <c r="K1487" t="inlineStr">
+        <is>
+          <t>미지정</t>
+        </is>
+      </c>
       <c r="L1487" t="inlineStr">
         <is>
           <t>인문사회대학</t>

</xml_diff>